<commit_message>
werking van puppet/ansible + profiel puppet en ansible terug toegevoegd (maar bij methodologie)
</commit_message>
<xml_diff>
--- a/R/deploytimes/deploytimes  (Automatisch opgeslagen).xlsx
+++ b/R/deploytimes/deploytimes  (Automatisch opgeslagen).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Puppet" sheetId="1" r:id="rId1"/>
@@ -727,11 +727,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1544577648"/>
-        <c:axId val="1544579968"/>
+        <c:axId val="-2146293392"/>
+        <c:axId val="-2146291072"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1544577648"/>
+        <c:axId val="-2146293392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +773,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1544579968"/>
+        <c:crossAx val="-2146291072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -781,7 +781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1544579968"/>
+        <c:axId val="-2146291072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +831,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1544577648"/>
+        <c:crossAx val="-2146293392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1126,11 +1126,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1544598848"/>
-        <c:axId val="1544601168"/>
+        <c:axId val="-2146267616"/>
+        <c:axId val="-2146264832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1544598848"/>
+        <c:axId val="-2146267616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1172,7 +1172,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1544601168"/>
+        <c:crossAx val="-2146264832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1180,7 +1180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1544601168"/>
+        <c:axId val="-2146264832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="30.0"/>
@@ -1231,7 +1231,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1544598848"/>
+        <c:crossAx val="-2146267616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1352,6 +1352,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1641,11 +1642,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1472822704"/>
-        <c:axId val="1472827216"/>
+        <c:axId val="-2146226448"/>
+        <c:axId val="-2146223696"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1472822704"/>
+        <c:axId val="-2146226448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1687,7 +1688,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1472827216"/>
+        <c:crossAx val="-2146223696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1695,7 +1696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1472827216"/>
+        <c:axId val="-2146223696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,7 +1746,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1472822704"/>
+        <c:crossAx val="-2146226448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1759,6 +1760,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1871,6 +1873,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2138,11 +2141,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1472870400"/>
-        <c:axId val="1472872176"/>
+        <c:axId val="-2146191040"/>
+        <c:axId val="-2146188288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1472870400"/>
+        <c:axId val="-2146191040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2184,7 +2187,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1472872176"/>
+        <c:crossAx val="-2146188288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2192,7 +2195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1472872176"/>
+        <c:axId val="-2146188288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,6 +2216,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2272,7 +2276,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1472870400"/>
+        <c:crossAx val="-2146191040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2286,6 +2290,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2392,6 +2397,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2614,11 +2620,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1544616592"/>
-        <c:axId val="1544619344"/>
+        <c:axId val="-2146161600"/>
+        <c:axId val="-2146158848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1544616592"/>
+        <c:axId val="-2146161600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2660,7 +2666,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1544619344"/>
+        <c:crossAx val="-2146158848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2668,7 +2674,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1544619344"/>
+        <c:axId val="-2146158848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2689,6 +2695,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2748,7 +2755,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1544616592"/>
+        <c:crossAx val="-2146161600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2762,6 +2769,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6110,7 +6118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
@@ -6890,7 +6898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
@@ -7476,10 +7484,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7487,7 +7495,7 @@
     <col min="2" max="2" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>23</v>
       </c>
@@ -7498,59 +7506,56 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="9">
-        <f>AVERAGE(Ansible!B6:U6)</f>
-        <v>6.25</v>
+        <f>AVERAGE(Ansible!B6:AE6)</f>
+        <v>6.5666666666666664</v>
       </c>
       <c r="D2" s="9">
-        <f>AVERAGE(Tabel1[[#This Row],[1]:[20]])</f>
-        <v>7.5545</v>
+        <f>AVERAGE(Tabel1[[#This Row],[1]:[30]])</f>
+        <v>8.2696666666666676</v>
+      </c>
+      <c r="E2">
+        <v>7.6</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="9">
-        <f>STDEV(Ansible!B6:U6)</f>
-        <v>2.1244194253340942</v>
-      </c>
-      <c r="D3" s="9">
-        <f>STDEV(Puppet!B2:U2)</f>
-        <v>1.4570282481096533</v>
-      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="9">
-        <f>AVERAGE(Ansible!B7:U7)</f>
-        <v>56.95</v>
+        <f>AVERAGE(Ansible!B7:AE7)</f>
+        <v>60.666666666666664</v>
       </c>
       <c r="D4" s="9">
-        <f>AVERAGE(Puppet!B5:U5)</f>
-        <v>47.063500000000012</v>
+        <f>AVERAGE(Puppet!B5:AE5)</f>
+        <v>49.385333333333328</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="9">
-        <f>STDEV(Ansible!B7:U7)</f>
-        <v>9.9444509784682307</v>
+        <f>STDEV(Ansible!B7:AE7)</f>
+        <v>11.50212374193187</v>
       </c>
       <c r="D5" s="9">
-        <f>STDEV(Puppet!B5:U5)</f>
-        <v>13.302964558797811</v>
+        <f>STDEV(Tabel1[[#This Row],[1]:[30]])</f>
+        <v>11.566646977359124</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>46</v>
       </c>

</xml_diff>